<commit_message>
feat(load-data):shows info when uploading a file
</commit_message>
<xml_diff>
--- a/follow_students/static/excel_format/format.xlsx
+++ b/follow_students/static/excel_format/format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darwin Lenis\OneDrive\Escritorio\Universidad\5to Semestre\Proyecto Integrador\GitHub\Final-Project\follow_students\static\excel_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864141D2-0C79-4C72-927B-45B5418BC836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B2412F-4214-4EBF-844F-D8E677DAE3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37C6A70E-0892-4DA6-B95F-1D86B2DF07FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{37C6A70E-0892-4DA6-B95F-1D86B2DF07FB}"/>
   </bookViews>
   <sheets>
     <sheet name="_x0009_MAT-08273" sheetId="2" r:id="rId1"/>
@@ -225,17 +225,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -552,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7610B327-885F-4AAB-9C7A-CE572AFDF5EC}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,8 +566,6 @@
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -577,8 +574,8 @@
       <c r="B2" s="2">
         <v>1.83</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -587,8 +584,8 @@
       <c r="B3" s="2">
         <v>1.32</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -597,8 +594,8 @@
       <c r="B4" s="2">
         <v>1.73</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -607,8 +604,8 @@
       <c r="B5" s="2">
         <v>1.1399999999999999</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -617,8 +614,8 @@
       <c r="B6" s="2">
         <v>1.35</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -627,8 +624,8 @@
       <c r="B7" s="2">
         <v>1.32</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -637,8 +634,8 @@
       <c r="B8" s="2">
         <v>1.65</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -647,8 +644,8 @@
       <c r="B9" s="2">
         <v>1.2</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -657,8 +654,8 @@
       <c r="B10" s="2">
         <v>1.5</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -667,8 +664,8 @@
       <c r="B11" s="2">
         <v>1.7</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -677,8 +674,8 @@
       <c r="B12" s="2">
         <v>1.39</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -687,8 +684,8 @@
       <c r="B13" s="2">
         <v>1.05</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -697,8 +694,8 @@
       <c r="B14" s="2">
         <v>1.55</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -707,8 +704,8 @@
       <c r="B15" s="2">
         <v>1.65</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -717,169 +714,168 @@
       <c r="B16" s="2">
         <v>1.37</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2">
         <v>1.3</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2">
         <v>1.32</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2">
         <v>1.17</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2">
         <v>1.21</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>0.91</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2">
         <v>1.62</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="2">
         <v>1.52</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2">
         <v>1.73</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="2">
         <v>1.24</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="2">
         <v>1.22</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="2">
         <v>0.97</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="2">
         <v>1.83</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="2">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="2">
         <v>1.55</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="2">
         <v>0.98</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -888,8 +884,8 @@
       <c r="B33" s="2">
         <v>1.37</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -898,8 +894,8 @@
       <c r="B34" s="2">
         <v>1.21</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -908,8 +904,8 @@
       <c r="B35" s="2">
         <v>1.76</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -918,8 +914,8 @@
       <c r="B36" s="2">
         <v>1.36</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -928,8 +924,8 @@
       <c r="B37" s="2">
         <v>1.5</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -938,24 +934,8 @@
       <c r="B38" s="2">
         <v>1.5</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -964,10 +944,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF789E85-769D-4EA3-94AE-AA3E51CDE9C9}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,8 +959,6 @@
       <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -989,8 +967,8 @@
       <c r="B2" s="2">
         <v>1.83</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -999,8 +977,8 @@
       <c r="B3" s="2">
         <v>1.32</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1009,8 +987,8 @@
       <c r="B4" s="2">
         <v>1.73</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1019,8 +997,8 @@
       <c r="B5" s="2">
         <v>1.1399999999999999</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1029,8 +1007,8 @@
       <c r="B6" s="2">
         <v>1.35</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1039,8 +1017,8 @@
       <c r="B7" s="2">
         <v>1.32</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1049,8 +1027,8 @@
       <c r="B8" s="2">
         <v>1.65</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1059,8 +1037,8 @@
       <c r="B9" s="2">
         <v>1.2</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1069,8 +1047,8 @@
       <c r="B10" s="2">
         <v>1.5</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1079,8 +1057,8 @@
       <c r="B11" s="2">
         <v>1.7</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1089,8 +1067,8 @@
       <c r="B12" s="2">
         <v>1.39</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1099,8 +1077,8 @@
       <c r="B13" s="2">
         <v>1.05</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1109,8 +1087,8 @@
       <c r="B14" s="2">
         <v>1.55</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1119,8 +1097,8 @@
       <c r="B15" s="2">
         <v>1.65</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1129,168 +1107,169 @@
       <c r="B16" s="2">
         <v>1.37</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="2">
         <v>1.3</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2">
         <v>1.32</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2">
         <v>1.17</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2">
         <v>1.21</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>0.91</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2">
         <v>1.62</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="2">
         <v>1.52</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2">
         <v>1.73</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="2">
         <v>1.24</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="2">
         <v>1.22</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="2">
         <v>0.97</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="2">
         <v>1.83</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="2">
         <v>1.1499999999999999</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="2">
         <v>1.55</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="2">
         <v>0.98</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -1299,8 +1278,8 @@
       <c r="B33" s="2">
         <v>1.37</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -1309,8 +1288,8 @@
       <c r="B34" s="2">
         <v>1.21</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -1319,8 +1298,8 @@
       <c r="B35" s="2">
         <v>1.76</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -1329,8 +1308,8 @@
       <c r="B36" s="2">
         <v>1.36</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -1339,8 +1318,8 @@
       <c r="B37" s="2">
         <v>1.5</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -1349,24 +1328,8 @@
       <c r="B38" s="2">
         <v>1.5</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2017,7 +1980,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2596,7 +2559,7 @@
       <c r="B32" s="2">
         <v>0.98</v>
       </c>
-      <c r="L32" s="6"/>
+      <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">

</xml_diff>